<commit_message>
added refresh, fixed data issue
Changed all the values in source xlsx to 'text' and that fixed the date conversion issue we were seeing.
</commit_message>
<xml_diff>
--- a/Examples/ProjectManagement/tasks.xlsx
+++ b/Examples/ProjectManagement/tasks.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\ProjectFrelard\Samples\ProjectManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bklower\Documents\GitHub\ProjectFrelard\Examples\ProjectManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="13815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19200"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="77">
   <si>
     <t>Assigned</t>
   </si>
@@ -46,18 +45,45 @@
     <t>GIF</t>
   </si>
   <si>
+    <t>2017-04-22</t>
+  </si>
+  <si>
+    <t>2017-4-26</t>
+  </si>
+  <si>
+    <t>2017-4-23</t>
+  </si>
+  <si>
+    <t>2017-4-25</t>
+  </si>
+  <si>
     <t>Emily</t>
   </si>
   <si>
     <t>Blog post</t>
   </si>
   <si>
+    <t>2017-5-4</t>
+  </si>
+  <si>
+    <t>2017-5-8</t>
+  </si>
+  <si>
+    <t>2017-5-11</t>
+  </si>
+  <si>
     <t>Stephanie</t>
   </si>
   <si>
     <t>CSS</t>
   </si>
   <si>
+    <t>2017-5-1</t>
+  </si>
+  <si>
+    <t>2017-5-10</t>
+  </si>
+  <si>
     <t>Piper</t>
   </si>
   <si>
@@ -70,31 +96,160 @@
     <t>Kevin</t>
   </si>
   <si>
+    <t>2017-5-20</t>
+  </si>
+  <si>
+    <t>2017-5-22</t>
+  </si>
+  <si>
     <t>Jordan</t>
   </si>
   <si>
     <t>Workbook</t>
   </si>
   <si>
+    <t>2017-4-22</t>
+  </si>
+  <si>
+    <t>2017-5-25</t>
+  </si>
+  <si>
+    <t>2017-5-21</t>
+  </si>
+  <si>
+    <t>2017-6-2</t>
+  </si>
+  <si>
     <t>Tracy</t>
   </si>
   <si>
     <t>Video</t>
   </si>
   <si>
+    <t>2017-5-27</t>
+  </si>
+  <si>
+    <t>2017-6-3</t>
+  </si>
+  <si>
+    <t>2017-6-10</t>
+  </si>
+  <si>
+    <t>2017-5-19</t>
+  </si>
+  <si>
+    <t>2017-6-15</t>
+  </si>
+  <si>
+    <t>2017-6-22</t>
+  </si>
+  <si>
+    <t>2017-6-18</t>
+  </si>
+  <si>
+    <t>2017-6-28</t>
+  </si>
+  <si>
     <t>Webpage</t>
   </si>
   <si>
+    <t>2017-6-25</t>
+  </si>
+  <si>
     <t>Viz</t>
   </si>
   <si>
+    <t>2017-4-20</t>
+  </si>
+  <si>
+    <t>2017-7-1</t>
+  </si>
+  <si>
+    <t>2017-6-30</t>
+  </si>
+  <si>
+    <t>2017-7-3</t>
+  </si>
+  <si>
+    <t>2017-7-6</t>
+  </si>
+  <si>
     <t>Marissa</t>
   </si>
   <si>
+    <t>2017-7-7</t>
+  </si>
+  <si>
     <t>Mike</t>
   </si>
   <si>
+    <t>2017-7-16</t>
+  </si>
+  <si>
+    <t>2017-7-2</t>
+  </si>
+  <si>
+    <t>2017-7-17</t>
+  </si>
+  <si>
+    <t>2017-07-02</t>
+  </si>
+  <si>
+    <t>2017-08-02</t>
+  </si>
+  <si>
+    <t>2017-7-14</t>
+  </si>
+  <si>
+    <t>2017-7-20</t>
+  </si>
+  <si>
+    <t>2017-7-22</t>
+  </si>
+  <si>
+    <t>2017-7-18</t>
+  </si>
+  <si>
+    <t>2017-7-28</t>
+  </si>
+  <si>
+    <t>2017-7-15</t>
+  </si>
+  <si>
+    <t>2017-8-4</t>
+  </si>
+  <si>
+    <t>2017-8-2</t>
+  </si>
+  <si>
+    <t>2017-08-15</t>
+  </si>
+  <si>
     <t>Slideshare</t>
+  </si>
+  <si>
+    <t>2017-3-20</t>
+  </si>
+  <si>
+    <t>2017-8-19</t>
+  </si>
+  <si>
+    <t>2017-8-11</t>
+  </si>
+  <si>
+    <t>2017-9-22</t>
+  </si>
+  <si>
+    <t>2017-9-24</t>
+  </si>
+  <si>
+    <t>2017-7-10</t>
+  </si>
+  <si>
+    <t>2017-10-2</t>
+  </si>
+  <si>
+    <t>2017-10-3</t>
   </si>
 </sst>
 </file>
@@ -132,7 +287,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,12 +631,12 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E31"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -512,14 +667,14 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
-        <v>42847</v>
-      </c>
-      <c r="D2" s="1">
-        <v>42851</v>
-      </c>
-      <c r="E2" s="1">
-        <v>42851</v>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -532,14 +687,14 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>42848</v>
-      </c>
-      <c r="D3" s="1">
-        <v>42851</v>
-      </c>
-      <c r="E3" s="1">
-        <v>42850</v>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -547,19 +702,19 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>42859</v>
-      </c>
-      <c r="D4" s="1">
-        <v>42863</v>
-      </c>
-      <c r="E4" s="1">
-        <v>42866</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -567,19 +722,19 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>42856</v>
-      </c>
-      <c r="D5" s="1">
-        <v>42865</v>
-      </c>
-      <c r="E5" s="1">
-        <v>42865</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -587,19 +742,19 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1">
-        <v>42856</v>
-      </c>
-      <c r="D6" s="1">
-        <v>42865</v>
-      </c>
-      <c r="E6" s="1">
-        <v>42865</v>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -607,19 +762,19 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1">
-        <v>42856</v>
-      </c>
-      <c r="D7" s="1">
-        <v>42865</v>
-      </c>
-      <c r="E7" s="1">
-        <v>42866</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -627,19 +782,19 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
-        <v>42875</v>
-      </c>
-      <c r="D8" s="1">
-        <v>42875</v>
-      </c>
-      <c r="E8" s="1">
-        <v>42877</v>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -647,19 +802,19 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1">
-        <v>42847</v>
-      </c>
-      <c r="D9" s="1">
-        <v>42877</v>
-      </c>
-      <c r="E9" s="1">
-        <v>42877</v>
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -667,19 +822,19 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1">
-        <v>42863</v>
-      </c>
-      <c r="D10" s="1">
-        <v>42880</v>
-      </c>
-      <c r="E10" s="1">
-        <v>42880</v>
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -687,19 +842,19 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
-        <v>42876</v>
-      </c>
-      <c r="D11" s="1">
-        <v>42888</v>
-      </c>
-      <c r="E11" s="1">
-        <v>42888</v>
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -707,19 +862,19 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1">
-        <v>42882</v>
-      </c>
-      <c r="D12" s="1">
-        <v>42889</v>
-      </c>
-      <c r="E12" s="1">
-        <v>42889</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F12">
         <v>11</v>
@@ -727,19 +882,19 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
-        <v>42888</v>
-      </c>
-      <c r="D13" s="1">
-        <v>42896</v>
-      </c>
-      <c r="E13" s="1">
-        <v>42896</v>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F13">
         <v>12</v>
@@ -747,19 +902,19 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1">
-        <v>42874</v>
-      </c>
-      <c r="D14" s="1">
-        <v>42901</v>
-      </c>
-      <c r="E14" s="1">
-        <v>42901</v>
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -767,19 +922,19 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>42888</v>
-      </c>
-      <c r="D15" s="1">
-        <v>42908</v>
-      </c>
-      <c r="E15" s="1">
-        <v>42908</v>
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -787,19 +942,19 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1">
-        <v>42904</v>
-      </c>
-      <c r="D16" s="1">
-        <v>42914</v>
-      </c>
-      <c r="E16" s="1">
-        <v>42914</v>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -810,16 +965,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1">
-        <v>42911</v>
-      </c>
-      <c r="D17" s="1">
-        <v>42914</v>
-      </c>
-      <c r="E17" s="1">
-        <v>42914</v>
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F17">
         <v>16</v>
@@ -827,19 +982,19 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1">
-        <v>42845</v>
-      </c>
-      <c r="D18" s="1">
-        <v>42917</v>
-      </c>
-      <c r="E18" s="1">
-        <v>42917</v>
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F18">
         <v>17</v>
@@ -847,19 +1002,19 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="1">
-        <v>42916</v>
-      </c>
-      <c r="D19" s="1">
-        <v>42919</v>
-      </c>
-      <c r="E19" s="1">
-        <v>42922</v>
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="F19">
         <v>18</v>
@@ -867,19 +1022,19 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="1">
-        <v>42916</v>
-      </c>
-      <c r="D20" s="1">
-        <v>42923</v>
-      </c>
-      <c r="E20" s="1">
-        <v>42923</v>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="F20">
         <v>19</v>
@@ -887,19 +1042,19 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1">
-        <v>42932</v>
-      </c>
-      <c r="D21" s="1">
-        <v>42932</v>
-      </c>
-      <c r="E21" s="1">
-        <v>42932</v>
+        <v>13</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F21">
         <v>20</v>
@@ -907,19 +1062,19 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="1">
-        <v>42918</v>
-      </c>
-      <c r="D22" s="1">
-        <v>42933</v>
-      </c>
-      <c r="E22" s="1">
-        <v>42933</v>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="F22">
         <v>21</v>
@@ -927,19 +1082,19 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1">
-        <v>42901</v>
-      </c>
-      <c r="D23" s="1">
-        <v>42936</v>
-      </c>
-      <c r="E23" s="1">
-        <v>42949</v>
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F23">
         <v>22</v>
@@ -947,19 +1102,19 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1">
-        <v>42930</v>
-      </c>
-      <c r="D24" s="1">
-        <v>42936</v>
-      </c>
-      <c r="E24" s="1">
-        <v>42938</v>
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F24">
         <v>23</v>
@@ -967,19 +1122,19 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="1">
-        <v>42934</v>
-      </c>
-      <c r="D25" s="1">
-        <v>42936</v>
-      </c>
-      <c r="E25" s="1">
-        <v>42936</v>
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F25">
         <v>24</v>
@@ -987,19 +1142,19 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="1">
-        <v>42933</v>
-      </c>
-      <c r="D26" s="1">
-        <v>42944</v>
-      </c>
-      <c r="E26" s="1">
-        <v>42944</v>
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F26">
         <v>25</v>
@@ -1007,19 +1162,19 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="1">
-        <v>42931</v>
-      </c>
-      <c r="D27" s="1">
-        <v>42951</v>
-      </c>
-      <c r="E27" s="1">
-        <v>42951</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="F27">
         <v>26</v>
@@ -1027,19 +1182,19 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="1">
-        <v>42949</v>
-      </c>
-      <c r="D28" s="1">
-        <v>42962</v>
-      </c>
-      <c r="E28" s="1">
-        <v>42962</v>
+        <v>23</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="F28">
         <v>27</v>
@@ -1047,19 +1202,19 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1">
-        <v>42814</v>
-      </c>
-      <c r="D29" s="1">
-        <v>42966</v>
-      </c>
-      <c r="E29" s="1">
-        <v>42966</v>
+        <v>68</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F29">
         <v>28</v>
@@ -1067,19 +1222,19 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="1">
-        <v>42958</v>
-      </c>
-      <c r="D30" s="1">
-        <v>43000</v>
-      </c>
-      <c r="E30" s="1">
-        <v>43002</v>
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F30">
         <v>29</v>
@@ -1087,19 +1242,19 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="1">
-        <v>42926</v>
-      </c>
-      <c r="D31" s="1">
-        <v>43010</v>
-      </c>
-      <c r="E31" s="1">
-        <v>43011</v>
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F31">
         <v>30</v>

</xml_diff>